<commit_message>
Single and Multi-question branching reading added
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0355957-6512-4755-BC08-8D0B97321732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436D607F-968B-4313-969F-5D6BCF932C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="554">
   <si>
     <t>Environment</t>
   </si>
@@ -1666,7 +1666,25 @@
     <t>PlatformReadings_TC71</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Advance Branching page - load (sid - 157) (Page 2)</t>
+  </si>
+  <si>
+    <t>Apply branching on 5 questions page 1 - save (sid - 157)</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC72</t>
+  </si>
+  <si>
+    <t>Multi-Question Branching</t>
+  </si>
+  <si>
+    <t>Single-Question Branching</t>
+  </si>
+  <si>
+    <t>Branching page - load (sid - 157) (Page 1)</t>
+  </si>
+  <si>
+    <t>Apply branching on 5 questions - Save (Take reading on 5th Save) (sid - 157)</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1692,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1787,46 +1805,9 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1862,7 +1843,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="74">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1962,183 +1943,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2286,7 +2092,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2319,38 +2125,19 @@
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="24" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="47" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="25" fillId="49" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="51" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="53" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="27" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="28" fillId="57" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="28" fillId="59" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="28" fillId="61" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="30" fillId="63" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="30" fillId="65" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="30" fillId="67" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="32" fillId="69" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="32" fillId="71" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="32" fillId="73" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2857,10 +2644,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C4B212-CB98-4DB5-B9D6-ACC2C7B6F74B}">
-  <dimension ref="A1:CK72"/>
+  <dimension ref="A1:CK73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K81" sqref="K81"/>
+    <sheetView tabSelected="1" topLeftCell="BV61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O73" sqref="O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11913,11 +11700,13 @@
       <c r="F72" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>550</v>
+      </c>
       <c r="H72" s="1"/>
       <c r="I72" s="11"/>
-      <c r="J72" s="59" t="s">
-        <v>547</v>
+      <c r="J72" s="30" t="s">
+        <v>526</v>
       </c>
       <c r="K72" s="16"/>
       <c r="L72" s="16" t="s">
@@ -11926,8 +11715,12 @@
       <c r="M72" s="16">
         <v>157</v>
       </c>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
+      <c r="N72" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>548</v>
+      </c>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -12003,6 +11796,121 @@
       <c r="CJ72" s="10"/>
       <c r="CK72" s="16"/>
     </row>
+    <row r="73" spans="1:89" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="H73" s="1"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16" t="s">
+        <v>480</v>
+      </c>
+      <c r="M73" s="16">
+        <v>157</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
+      <c r="AC73" s="1"/>
+      <c r="AD73" s="1"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="1"/>
+      <c r="AG73" s="1"/>
+      <c r="AH73" s="1"/>
+      <c r="AI73" s="1"/>
+      <c r="AJ73" s="1"/>
+      <c r="AK73" s="1"/>
+      <c r="AL73" s="1"/>
+      <c r="AM73" s="1"/>
+      <c r="AN73" s="1"/>
+      <c r="AO73" s="1"/>
+      <c r="AP73" s="1"/>
+      <c r="AQ73" s="1"/>
+      <c r="AR73" s="1"/>
+      <c r="AS73" s="1"/>
+      <c r="AT73" s="1"/>
+      <c r="AU73" s="1"/>
+      <c r="AV73" s="7"/>
+      <c r="AW73" s="1"/>
+      <c r="AX73" s="1"/>
+      <c r="AY73" s="1"/>
+      <c r="AZ73" s="1"/>
+      <c r="BA73" s="1"/>
+      <c r="BB73" s="1"/>
+      <c r="BC73" s="1"/>
+      <c r="BD73" s="1"/>
+      <c r="BE73" s="1"/>
+      <c r="BF73" s="1"/>
+      <c r="BG73" s="7"/>
+      <c r="BH73" s="1"/>
+      <c r="BI73" s="1"/>
+      <c r="BJ73" s="1"/>
+      <c r="BK73" s="1"/>
+      <c r="BL73" s="1"/>
+      <c r="BM73" s="1"/>
+      <c r="BN73" s="1"/>
+      <c r="BO73" s="1"/>
+      <c r="BP73" s="1"/>
+      <c r="BQ73" s="2"/>
+      <c r="BR73" s="8"/>
+      <c r="BS73" s="8"/>
+      <c r="BT73" s="8"/>
+      <c r="BU73" s="1"/>
+      <c r="BV73" s="1"/>
+      <c r="BW73" s="1"/>
+      <c r="BX73" s="1"/>
+      <c r="BY73" s="1"/>
+      <c r="BZ73" s="9"/>
+      <c r="CA73" s="9"/>
+      <c r="CB73" s="10"/>
+      <c r="CC73" s="10"/>
+      <c r="CD73" s="10"/>
+      <c r="CE73" s="14"/>
+      <c r="CF73" s="15"/>
+      <c r="CG73" s="10"/>
+      <c r="CH73" s="10"/>
+      <c r="CI73" s="10"/>
+      <c r="CJ73" s="10"/>
+      <c r="CK73" s="16"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Re-arrange question readings added
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABB709F-2F32-4A8D-8D7B-89FB3663ADAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BF56FF-CEEF-481C-9985-C9FA88E9D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="583">
   <si>
     <t>Environment</t>
   </si>
@@ -1438,30 +1438,6 @@
     <t>PlatformReadings_TC63</t>
   </si>
   <si>
-    <t>ML page - load(1487 Survey copied from )  (sid - 157)</t>
-  </si>
-  <si>
-    <t>Autotranslate all question and messages(Arabic language) - completion</t>
-  </si>
-  <si>
-    <t>Autotranslate all question and messages(Arabic language) - save</t>
-  </si>
-  <si>
-    <t>Autotranslate all question and messages(Arabic language) - reset</t>
-  </si>
-  <si>
-    <t>Spell check on Entire survey - load  (SID 157)</t>
-  </si>
-  <si>
-    <t>Spell check on Entire survey - save (SID 157)</t>
-  </si>
-  <si>
-    <t>Arabic</t>
-  </si>
-  <si>
-    <t>Readings - 20-Apr-2022 20:42:36</t>
-  </si>
-  <si>
     <t>PlatformReadings_TC64</t>
   </si>
   <si>
@@ -1585,12 +1561,6 @@
     <t>Survey Creation Readings</t>
   </si>
   <si>
-    <t>All question type readings</t>
-  </si>
-  <si>
-    <t>AutoTranslation Readings</t>
-  </si>
-  <si>
     <t>QDL Readings</t>
   </si>
   <si>
@@ -1681,39 +1651,9 @@
     <t>Apply branching on 5 questions - Save (Take reading on 5th Save) (sid - 157)</t>
   </si>
   <si>
-    <t>PlatformReadings_TC62.1</t>
-  </si>
-  <si>
     <t>Drop Down Question Readings</t>
   </si>
   <si>
-    <t>PlatformReadings_TC63_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC64_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC65_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC66_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC67_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC68_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC70_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC71_1</t>
-  </si>
-  <si>
-    <t>PlatformReadings_TC72_1</t>
-  </si>
-  <si>
     <t>Radio Button Question Readings</t>
   </si>
   <si>
@@ -1820,6 +1760,18 @@
   </si>
   <si>
     <t>PlatformReadings_TC91</t>
+  </si>
+  <si>
+    <t>PlatformReadings_TC82</t>
+  </si>
+  <si>
+    <t>Re-arrange Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rearrange page - load </t>
+  </si>
+  <si>
+    <t>Rearrange 10 questions - save  (sid - 157)</t>
   </si>
 </sst>
 </file>
@@ -1827,7 +1779,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1920,13 +1872,11 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1944,41 +1894,8 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="42">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2010,16 +1927,6 @@
     <fill>
       <patternFill patternType="none">
         <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
       </patternFill>
     </fill>
     <fill>
@@ -2068,93 +1975,13 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2242,7 +2069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2266,8 +2093,8 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2277,18 +2104,6 @@
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2599,7 +2414,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -2795,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C4B212-CB98-4DB5-B9D6-ACC2C7B6F74B}">
-  <dimension ref="A1:CK100"/>
+  <dimension ref="A1:CK91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N95" sqref="N95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,7 +2664,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>36</v>
@@ -3110,7 +2925,7 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="6"/>
@@ -3233,7 +3048,7 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K3" s="6"/>
@@ -3354,7 +3169,7 @@
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="6"/>
@@ -3475,7 +3290,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="12"/>
@@ -3596,7 +3411,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K6" s="12"/>
@@ -3733,7 +3548,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="12"/>
@@ -3870,7 +3685,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="12"/>
@@ -3993,7 +3808,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="12"/>
@@ -4118,7 +3933,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="11"/>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K10" s="12"/>
@@ -4243,7 +4058,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="11"/>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="12"/>
@@ -4368,7 +4183,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="11"/>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K12" s="12"/>
@@ -4493,7 +4308,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K13" s="12"/>
@@ -4620,7 +4435,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K14" s="12"/>
@@ -4747,7 +4562,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K15" s="12"/>
@@ -4868,7 +4683,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K16" s="12"/>
@@ -4981,7 +4796,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="11"/>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K17" s="12"/>
@@ -5104,7 +4919,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="11"/>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K18" s="12"/>
@@ -5229,7 +5044,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11"/>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K19" s="12"/>
@@ -5360,7 +5175,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="11"/>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K20" s="12"/>
@@ -5495,7 +5310,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K21" s="12"/>
@@ -5626,7 +5441,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K22" s="12"/>
@@ -5757,7 +5572,7 @@
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K23" s="12"/>
@@ -5880,7 +5695,7 @@
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K24" s="12"/>
@@ -6003,7 +5818,7 @@
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="11"/>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K25" s="12"/>
@@ -6134,7 +5949,7 @@
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="11"/>
-      <c r="J26" s="20" t="s">
+      <c r="J26" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K26" s="12"/>
@@ -6243,11 +6058,11 @@
         <v>340</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="11"/>
-      <c r="J27" s="20" t="s">
+      <c r="J27" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K27" s="12"/>
@@ -6335,7 +6150,7 @@
         <v>118</v>
       </c>
       <c r="BS27" s="8" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="BT27" s="8"/>
       <c r="BU27" s="1" t="s">
@@ -6378,11 +6193,11 @@
         <v>340</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="11"/>
-      <c r="J28" s="20" t="s">
+      <c r="J28" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K28" s="12"/>
@@ -6469,7 +6284,7 @@
       </c>
       <c r="BS28" s="8"/>
       <c r="BT28" s="8" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="BU28" s="1" t="s">
         <v>331</v>
@@ -6511,11 +6326,11 @@
         <v>340</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="20" t="s">
+      <c r="J29" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K29" s="12"/>
@@ -6602,7 +6417,7 @@
       </c>
       <c r="BS29" s="8"/>
       <c r="BT29" s="8" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="BU29" s="1" t="s">
         <v>331</v>
@@ -6644,11 +6459,11 @@
         <v>340</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="11"/>
-      <c r="J30" s="20" t="s">
+      <c r="J30" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K30" s="12"/>
@@ -6721,7 +6536,7 @@
       </c>
       <c r="BS30" s="8"/>
       <c r="BT30" s="8" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="BU30" s="1"/>
       <c r="BV30" s="1" t="s">
@@ -6767,7 +6582,7 @@
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="11"/>
-      <c r="J31" s="20" t="s">
+      <c r="J31" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K31" s="12"/>
@@ -6894,7 +6709,7 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="11"/>
-      <c r="J32" s="20" t="s">
+      <c r="J32" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K32" s="12"/>
@@ -7017,7 +6832,7 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" s="11"/>
-      <c r="J33" s="20" t="s">
+      <c r="J33" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K33" s="12"/>
@@ -7136,7 +6951,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="11"/>
-      <c r="J34" s="20" t="s">
+      <c r="J34" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K34" s="12"/>
@@ -7251,7 +7066,7 @@
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="11"/>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K35" s="12"/>
@@ -7366,7 +7181,7 @@
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="11"/>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K36" s="12"/>
@@ -7481,7 +7296,7 @@
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="11"/>
-      <c r="J37" s="20" t="s">
+      <c r="J37" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K37" s="12"/>
@@ -7596,7 +7411,7 @@
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="11"/>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K38" s="12"/>
@@ -7711,7 +7526,7 @@
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="11"/>
-      <c r="J39" s="20" t="s">
+      <c r="J39" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K39" s="12"/>
@@ -7826,7 +7641,7 @@
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="11"/>
-      <c r="J40" s="20" t="s">
+      <c r="J40" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K40" s="12"/>
@@ -7949,7 +7764,7 @@
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="11"/>
-      <c r="J41" s="20" t="s">
+      <c r="J41" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K41" s="12"/>
@@ -8066,7 +7881,7 @@
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="11"/>
-      <c r="J42" s="20" t="s">
+      <c r="J42" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K42" s="12"/>
@@ -8139,7 +7954,7 @@
       </c>
       <c r="BS42" s="8"/>
       <c r="BT42" s="8" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="BU42" s="1" t="s">
         <v>331</v>
@@ -8187,7 +8002,7 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="11"/>
-      <c r="J43" s="20" t="s">
+      <c r="J43" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K43" s="12"/>
@@ -8259,7 +8074,7 @@
         <v>118</v>
       </c>
       <c r="BS43" s="8" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="BT43" s="8"/>
       <c r="BU43" s="1" t="s">
@@ -8308,7 +8123,7 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="11"/>
-      <c r="J44" s="20" t="s">
+      <c r="J44" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K44" s="12"/>
@@ -8381,7 +8196,7 @@
       </c>
       <c r="BS44" s="8"/>
       <c r="BT44" s="8" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="BU44" s="1" t="s">
         <v>331</v>
@@ -8429,7 +8244,7 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="11"/>
-      <c r="J45" s="20" t="s">
+      <c r="J45" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K45" s="12"/>
@@ -8514,7 +8329,7 @@
       </c>
       <c r="BS45" s="8"/>
       <c r="BT45" s="8" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="BU45" s="1" t="s">
         <v>331</v>
@@ -8564,7 +8379,7 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="11"/>
-      <c r="J46" s="20" t="s">
+      <c r="J46" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K46" s="12"/>
@@ -8637,7 +8452,7 @@
       </c>
       <c r="BS46" s="8"/>
       <c r="BT46" s="8" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="BU46" s="1" t="s">
         <v>331</v>
@@ -8685,7 +8500,7 @@
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="11"/>
-      <c r="J47" s="20" t="s">
+      <c r="J47" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K47" s="12"/>
@@ -8800,7 +8615,7 @@
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="11"/>
-      <c r="J48" s="20" t="s">
+      <c r="J48" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K48" s="12"/>
@@ -8915,7 +8730,7 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="11"/>
-      <c r="J49" s="20" t="s">
+      <c r="J49" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K49" s="12"/>
@@ -9030,7 +8845,7 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="11"/>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="18" t="s">
         <v>26</v>
       </c>
       <c r="K50" s="12"/>
@@ -9155,7 +8970,7 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="11"/>
-      <c r="J51" s="19" t="s">
+      <c r="J51" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K51" s="12"/>
@@ -9276,7 +9091,7 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="11"/>
-      <c r="J52" s="19" t="s">
+      <c r="J52" s="17" t="s">
         <v>26</v>
       </c>
       <c r="K52" s="12"/>
@@ -9397,7 +9212,7 @@
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="11"/>
-      <c r="J53" s="21" t="s">
+      <c r="J53" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K53" s="16"/>
@@ -9512,7 +9327,7 @@
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="11"/>
-      <c r="J54" s="21" t="s">
+      <c r="J54" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K54" s="16"/>
@@ -9649,7 +9464,7 @@
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="11"/>
-      <c r="J55" s="21" t="s">
+      <c r="J55" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K55" s="16"/>
@@ -9786,7 +9601,7 @@
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="11"/>
-      <c r="J56" s="21" t="s">
+      <c r="J56" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K56" s="16"/>
@@ -9923,7 +9738,7 @@
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="11"/>
-      <c r="J57" s="21" t="s">
+      <c r="J57" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K57" s="16"/>
@@ -10060,7 +9875,7 @@
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="11"/>
-      <c r="J58" s="21" t="s">
+      <c r="J58" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K58" s="16"/>
@@ -10197,7 +10012,7 @@
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="11"/>
-      <c r="J59" s="21" t="s">
+      <c r="J59" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K59" s="16"/>
@@ -10334,7 +10149,7 @@
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="11"/>
-      <c r="J60" s="21" t="s">
+      <c r="J60" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K60" s="16"/>
@@ -10471,7 +10286,7 @@
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="11"/>
-      <c r="J61" s="21" t="s">
+      <c r="J61" s="19" t="s">
         <v>26</v>
       </c>
       <c r="K61" s="16"/>
@@ -10580,11 +10395,11 @@
         <v>399</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="11"/>
-      <c r="J62" s="42" t="s">
+      <c r="J62" s="26" t="s">
         <v>26</v>
       </c>
       <c r="K62" s="16"/>
@@ -10699,25 +10514,25 @@
         <v>399</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="11"/>
-      <c r="J63" s="23" t="s">
+      <c r="J63" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K63" s="16"/>
       <c r="L63" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M63" s="16">
         <v>157</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
@@ -10814,11 +10629,11 @@
         <v>399</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="11"/>
-      <c r="J64" s="23" t="s">
+      <c r="J64" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K64" s="16"/>
@@ -10911,7 +10726,7 @@
     </row>
     <row r="65" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>22</v>
@@ -10929,11 +10744,11 @@
         <v>399</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="11"/>
-      <c r="J65" s="23" t="s">
+      <c r="J65" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K65" s="16"/>
@@ -11026,7 +10841,7 @@
     </row>
     <row r="66" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>22</v>
@@ -11044,11 +10859,11 @@
         <v>399</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="11"/>
-      <c r="J66" s="23" t="s">
+      <c r="J66" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K66" s="16"/>
@@ -11141,7 +10956,7 @@
     </row>
     <row r="67" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>22</v>
@@ -11159,11 +10974,11 @@
         <v>399</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="11"/>
-      <c r="J67" s="23" t="s">
+      <c r="J67" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K67" s="16"/>
@@ -11256,7 +11071,7 @@
     </row>
     <row r="68" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>22</v>
@@ -11274,11 +11089,11 @@
         <v>399</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="11"/>
-      <c r="J68" s="23" t="s">
+      <c r="J68" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K68" s="16"/>
@@ -11371,7 +11186,7 @@
     </row>
     <row r="69" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>22</v>
@@ -11389,11 +11204,11 @@
         <v>399</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>577</v>
+        <v>557</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="11"/>
-      <c r="J69" s="23" t="s">
+      <c r="J69" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K69" s="16"/>
@@ -11486,7 +11301,7 @@
     </row>
     <row r="70" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>22</v>
@@ -11504,12 +11319,12 @@
         <v>399</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="11"/>
-      <c r="J70" s="24" t="s">
-        <v>525</v>
+      <c r="J70" s="22" t="s">
+        <v>515</v>
       </c>
       <c r="K70" s="16"/>
       <c r="L70" s="16" t="s">
@@ -11601,7 +11416,7 @@
     </row>
     <row r="71" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>22</v>
@@ -11619,12 +11434,12 @@
         <v>399</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="11"/>
-      <c r="J71" s="22" t="s">
-        <v>525</v>
+      <c r="J71" s="20" t="s">
+        <v>515</v>
       </c>
       <c r="K71" s="16"/>
       <c r="L71" s="16" t="s">
@@ -11716,7 +11531,7 @@
     </row>
     <row r="72" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>22</v>
@@ -11734,11 +11549,11 @@
         <v>399</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>580</v>
+        <v>560</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="11"/>
-      <c r="J72" s="23" t="s">
+      <c r="J72" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K72" s="16"/>
@@ -11831,7 +11646,7 @@
     </row>
     <row r="73" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>22</v>
@@ -11849,11 +11664,11 @@
         <v>399</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>579</v>
+        <v>559</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="11"/>
-      <c r="J73" s="23" t="s">
+      <c r="J73" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K73" s="16"/>
@@ -11946,7 +11761,7 @@
     </row>
     <row r="74" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>567</v>
+        <v>547</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>22</v>
@@ -11964,11 +11779,11 @@
         <v>399</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>576</v>
+        <v>556</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="11"/>
-      <c r="J74" s="23" t="s">
+      <c r="J74" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K74" s="16"/>
@@ -12061,7 +11876,7 @@
     </row>
     <row r="75" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>568</v>
+        <v>548</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>22</v>
@@ -12079,11 +11894,11 @@
         <v>399</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>581</v>
+        <v>561</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="11"/>
-      <c r="J75" s="23" t="s">
+      <c r="J75" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K75" s="16"/>
@@ -12176,7 +11991,7 @@
     </row>
     <row r="76" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>569</v>
+        <v>549</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>22</v>
@@ -12194,11 +12009,11 @@
         <v>399</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>582</v>
+        <v>562</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="11"/>
-      <c r="J76" s="23" t="s">
+      <c r="J76" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K76" s="16"/>
@@ -12291,7 +12106,7 @@
     </row>
     <row r="77" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>22</v>
@@ -12309,11 +12124,11 @@
         <v>399</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>583</v>
+        <v>563</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="11"/>
-      <c r="J77" s="23" t="s">
+      <c r="J77" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K77" s="16"/>
@@ -12406,7 +12221,7 @@
     </row>
     <row r="78" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>571</v>
+        <v>551</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>22</v>
@@ -12424,11 +12239,11 @@
         <v>399</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>584</v>
+        <v>564</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="11"/>
-      <c r="J78" s="23" t="s">
+      <c r="J78" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K78" s="16"/>
@@ -12521,7 +12336,7 @@
     </row>
     <row r="79" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>22</v>
@@ -12539,11 +12354,11 @@
         <v>399</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>585</v>
+        <v>565</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="11"/>
-      <c r="J79" s="23" t="s">
+      <c r="J79" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K79" s="16"/>
@@ -12636,7 +12451,7 @@
     </row>
     <row r="80" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>573</v>
+        <v>553</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>22</v>
@@ -12654,11 +12469,11 @@
         <v>399</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>586</v>
+        <v>566</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="11"/>
-      <c r="J80" s="23" t="s">
+      <c r="J80" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K80" s="16"/>
@@ -12751,7 +12566,7 @@
     </row>
     <row r="81" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>587</v>
+        <v>567</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>22</v>
@@ -12769,25 +12584,25 @@
         <v>399</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="11"/>
-      <c r="J81" s="25" t="s">
+      <c r="J81" s="23" t="s">
         <v>26</v>
       </c>
       <c r="K81" s="16"/>
       <c r="L81" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M81" s="16">
         <v>157</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
@@ -12866,7 +12681,7 @@
     </row>
     <row r="82" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>588</v>
+        <v>568</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>3</v>
@@ -12884,25 +12699,25 @@
         <v>399</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="11"/>
-      <c r="J82" s="23" t="s">
+      <c r="J82" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K82" s="16"/>
       <c r="L82" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M82" s="16">
         <v>157</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
@@ -12981,7 +12796,7 @@
     </row>
     <row r="83" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>3</v>
@@ -12999,25 +12814,25 @@
         <v>399</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>540</v>
+        <v>580</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="11"/>
-      <c r="J83" s="23" t="s">
-        <v>26</v>
+      <c r="J83" s="28" t="s">
+        <v>515</v>
       </c>
       <c r="K83" s="16"/>
       <c r="L83" s="16" t="s">
-        <v>543</v>
+        <v>472</v>
       </c>
       <c r="M83" s="16">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>541</v>
+        <v>581</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>542</v>
+        <v>582</v>
       </c>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
@@ -13096,10 +12911,10 @@
     </row>
     <row r="84" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>21</v>
@@ -13114,35 +12929,29 @@
         <v>399</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="11"/>
-      <c r="J84" s="23" t="s">
+      <c r="J84" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K84" s="16"/>
       <c r="L84" s="16" t="s">
-        <v>480</v>
+        <v>533</v>
       </c>
       <c r="M84" s="16">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>481</v>
+        <v>531</v>
       </c>
       <c r="O84" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="P84" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="Q84" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="R84" s="1" t="s">
-        <v>485</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
@@ -13173,18 +12982,10 @@
       <c r="AT84" s="1"/>
       <c r="AU84" s="1"/>
       <c r="AV84" s="7"/>
-      <c r="AW84" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AX84" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AY84" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AZ84" s="1" t="s">
-        <v>486</v>
-      </c>
+      <c r="AW84" s="1"/>
+      <c r="AX84" s="1"/>
+      <c r="AY84" s="1"/>
+      <c r="AZ84" s="1"/>
       <c r="BA84" s="1"/>
       <c r="BB84" s="1"/>
       <c r="BC84" s="1"/>
@@ -13197,9 +12998,7 @@
       <c r="BJ84" s="1"/>
       <c r="BK84" s="1"/>
       <c r="BL84" s="1"/>
-      <c r="BM84" s="1">
-        <v>19</v>
-      </c>
+      <c r="BM84" s="1"/>
       <c r="BN84" s="1"/>
       <c r="BO84" s="1"/>
       <c r="BP84" s="1"/>
@@ -13227,7 +13026,7 @@
     </row>
     <row r="85" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>22</v>
@@ -13245,29 +13044,35 @@
         <v>399</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="11"/>
-      <c r="J85" s="23" t="s">
+      <c r="J85" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K85" s="16"/>
       <c r="L85" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M85" s="16">
         <v>157</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
+        <v>474</v>
+      </c>
+      <c r="P85" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q85" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="R85" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
@@ -13298,10 +13103,18 @@
       <c r="AT85" s="1"/>
       <c r="AU85" s="1"/>
       <c r="AV85" s="7"/>
-      <c r="AW85" s="1"/>
-      <c r="AX85" s="1"/>
-      <c r="AY85" s="1"/>
-      <c r="AZ85" s="1"/>
+      <c r="AW85" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AX85" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AY85" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="AZ85" s="1" t="s">
+        <v>478</v>
+      </c>
       <c r="BA85" s="1"/>
       <c r="BB85" s="1"/>
       <c r="BC85" s="1"/>
@@ -13314,7 +13127,9 @@
       <c r="BJ85" s="1"/>
       <c r="BK85" s="1"/>
       <c r="BL85" s="1"/>
-      <c r="BM85" s="1"/>
+      <c r="BM85" s="1">
+        <v>19</v>
+      </c>
       <c r="BN85" s="1"/>
       <c r="BO85" s="1"/>
       <c r="BP85" s="1"/>
@@ -13329,9 +13144,7 @@
       <c r="BY85" s="1"/>
       <c r="BZ85" s="9"/>
       <c r="CA85" s="9"/>
-      <c r="CB85" s="10" t="s">
-        <v>518</v>
-      </c>
+      <c r="CB85" s="10"/>
       <c r="CC85" s="10"/>
       <c r="CD85" s="10"/>
       <c r="CE85" s="14"/>
@@ -13344,10 +13157,10 @@
     </row>
     <row r="86" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>592</v>
+        <v>571</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>21</v>
@@ -13362,41 +13175,31 @@
         <v>399</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="11"/>
-      <c r="J86" s="27" t="s">
-        <v>525</v>
+      <c r="J86" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="K86" s="16"/>
       <c r="L86" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M86" s="16">
         <v>157</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="P86" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="Q86" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="R86" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="S86" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="T86" s="1" t="s">
         <v>509</v>
       </c>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
@@ -13456,7 +13259,9 @@
       <c r="BY86" s="1"/>
       <c r="BZ86" s="9"/>
       <c r="CA86" s="9"/>
-      <c r="CB86" s="10"/>
+      <c r="CB86" s="10" t="s">
+        <v>510</v>
+      </c>
       <c r="CC86" s="10"/>
       <c r="CD86" s="10"/>
       <c r="CE86" s="14"/>
@@ -13469,10 +13274,10 @@
     </row>
     <row r="87" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>593</v>
+        <v>572</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>21</v>
@@ -13487,31 +13292,41 @@
         <v>399</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>596</v>
+        <v>494</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="11"/>
-      <c r="J87" s="23" t="s">
-        <v>26</v>
+      <c r="J87" s="25" t="s">
+        <v>515</v>
       </c>
       <c r="K87" s="16"/>
       <c r="L87" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M87" s="16">
         <v>157</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="P87" s="1"/>
-      <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
-      <c r="S87" s="1"/>
-      <c r="T87" s="1"/>
+        <v>500</v>
+      </c>
+      <c r="P87" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q87" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="R87" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="S87" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="T87" s="1" t="s">
+        <v>501</v>
+      </c>
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
@@ -13584,7 +13399,7 @@
     </row>
     <row r="88" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>22</v>
@@ -13602,25 +13417,25 @@
         <v>399</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>511</v>
+        <v>576</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="11"/>
-      <c r="J88" s="26" t="s">
-        <v>525</v>
+      <c r="J88" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="K88" s="16"/>
       <c r="L88" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M88" s="16">
         <v>157</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>512</v>
+        <v>482</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
@@ -13699,7 +13514,7 @@
     </row>
     <row r="89" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>595</v>
+        <v>574</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>22</v>
@@ -13717,32 +13532,28 @@
         <v>399</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>597</v>
+        <v>503</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="11"/>
-      <c r="J89" s="23" t="s">
-        <v>26</v>
+      <c r="J89" s="24" t="s">
+        <v>515</v>
       </c>
       <c r="K89" s="16"/>
       <c r="L89" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M89" s="16">
         <v>157</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="P89" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="Q89" s="1" t="s">
-        <v>495</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
@@ -13818,7 +13629,7 @@
     </row>
     <row r="90" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>598</v>
+        <v>575</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>22</v>
@@ -13836,30 +13647,32 @@
         <v>399</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>500</v>
+        <v>577</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="11"/>
-      <c r="J90" s="23" t="s">
+      <c r="J90" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K90" s="16"/>
       <c r="L90" s="16" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="M90" s="16">
         <v>157</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q90" s="1"/>
+        <v>486</v>
+      </c>
+      <c r="Q90" s="1" t="s">
+        <v>487</v>
+      </c>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
@@ -13935,7 +13748,7 @@
     </row>
     <row r="91" spans="1:89" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>552</v>
+        <v>578</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>22</v>
@@ -13953,122 +13766,60 @@
         <v>399</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="11"/>
-      <c r="J91" s="17" t="s">
-        <v>525</v>
+      <c r="J91" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="K91" s="16"/>
       <c r="L91" s="16" t="s">
-        <v>410</v>
+        <v>472</v>
       </c>
       <c r="M91" s="16">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>411</v>
+        <v>489</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>412</v>
+        <v>490</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="Q91" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="R91" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="S91" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="T91" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="U91" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="V91" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="W91" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="X91" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="Y91" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="Z91" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="AA91" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="AB91" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="AC91" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="AD91" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="AE91" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="AF91" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="AG91" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AH91" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="AI91" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="AJ91" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="AK91" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="AL91" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="AM91" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="AN91" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="AO91" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="AP91" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="AQ91" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="AR91" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="AS91" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="AT91" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="AU91" s="1" t="s">
-        <v>467</v>
-      </c>
+        <v>491</v>
+      </c>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+      <c r="AA91" s="1"/>
+      <c r="AB91" s="1"/>
+      <c r="AC91" s="1"/>
+      <c r="AD91" s="1"/>
+      <c r="AE91" s="1"/>
+      <c r="AF91" s="1"/>
+      <c r="AG91" s="1"/>
+      <c r="AH91" s="1"/>
+      <c r="AI91" s="1"/>
+      <c r="AJ91" s="1"/>
+      <c r="AK91" s="1"/>
+      <c r="AL91" s="1"/>
+      <c r="AM91" s="1"/>
+      <c r="AN91" s="1"/>
+      <c r="AO91" s="1"/>
+      <c r="AP91" s="1"/>
+      <c r="AQ91" s="1"/>
+      <c r="AR91" s="1"/>
+      <c r="AS91" s="1"/>
+      <c r="AT91" s="1"/>
+      <c r="AU91" s="1"/>
       <c r="AV91" s="7"/>
       <c r="AW91" s="1"/>
       <c r="AX91" s="1"/>
@@ -14112,1093 +13863,6 @@
       <c r="CJ91" s="10"/>
       <c r="CK91" s="16"/>
     </row>
-    <row r="92" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="H92" s="1"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16" t="s">
-        <v>478</v>
-      </c>
-      <c r="M92" s="16">
-        <v>185</v>
-      </c>
-      <c r="N92" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="O92" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="P92" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="Q92" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="R92" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="S92" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="T92" s="1"/>
-      <c r="U92" s="1"/>
-      <c r="V92" s="1"/>
-      <c r="W92" s="1"/>
-      <c r="X92" s="1"/>
-      <c r="Y92" s="1"/>
-      <c r="Z92" s="1"/>
-      <c r="AA92" s="1"/>
-      <c r="AB92" s="1"/>
-      <c r="AC92" s="1"/>
-      <c r="AD92" s="1"/>
-      <c r="AE92" s="1"/>
-      <c r="AF92" s="1"/>
-      <c r="AG92" s="1"/>
-      <c r="AH92" s="1"/>
-      <c r="AI92" s="1"/>
-      <c r="AJ92" s="1"/>
-      <c r="AK92" s="1"/>
-      <c r="AL92" s="1"/>
-      <c r="AM92" s="1"/>
-      <c r="AN92" s="1"/>
-      <c r="AO92" s="1"/>
-      <c r="AP92" s="1"/>
-      <c r="AQ92" s="1"/>
-      <c r="AR92" s="1"/>
-      <c r="AS92" s="1"/>
-      <c r="AT92" s="1"/>
-      <c r="AU92" s="1"/>
-      <c r="AV92" s="7"/>
-      <c r="AW92" s="1"/>
-      <c r="AX92" s="1"/>
-      <c r="AY92" s="1"/>
-      <c r="AZ92" s="1"/>
-      <c r="BA92" s="1"/>
-      <c r="BB92" s="1"/>
-      <c r="BC92" s="1"/>
-      <c r="BD92" s="1"/>
-      <c r="BE92" s="1"/>
-      <c r="BF92" s="1"/>
-      <c r="BG92" s="7"/>
-      <c r="BH92" s="1"/>
-      <c r="BI92" s="1"/>
-      <c r="BJ92" s="1"/>
-      <c r="BK92" s="1"/>
-      <c r="BL92" s="1"/>
-      <c r="BM92" s="1"/>
-      <c r="BN92" s="1"/>
-      <c r="BO92" s="1"/>
-      <c r="BP92" s="1"/>
-      <c r="BQ92" s="2"/>
-      <c r="BR92" s="8"/>
-      <c r="BS92" s="8"/>
-      <c r="BT92" s="8"/>
-      <c r="BU92" s="1"/>
-      <c r="BV92" s="1"/>
-      <c r="BW92" s="1"/>
-      <c r="BX92" s="1"/>
-      <c r="BY92" s="1"/>
-      <c r="BZ92" s="9"/>
-      <c r="CA92" s="9"/>
-      <c r="CB92" s="10"/>
-      <c r="CC92" s="10"/>
-      <c r="CD92" s="10"/>
-      <c r="CE92" s="14"/>
-      <c r="CF92" s="15"/>
-      <c r="CG92" s="10"/>
-      <c r="CH92" s="10"/>
-      <c r="CI92" s="10"/>
-      <c r="CJ92" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="CK92" s="16"/>
-    </row>
-    <row r="93" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="H93" s="1"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K93" s="16"/>
-      <c r="L93" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M93" s="16">
-        <v>157</v>
-      </c>
-      <c r="N93" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="O93" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="P93" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="Q93" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="R93" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="S93" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="T93" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="U93" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="V93" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="W93" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="X93" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="Y93" s="1"/>
-      <c r="Z93" s="1"/>
-      <c r="AA93" s="1"/>
-      <c r="AB93" s="1"/>
-      <c r="AC93" s="1"/>
-      <c r="AD93" s="1"/>
-      <c r="AE93" s="1"/>
-      <c r="AF93" s="1"/>
-      <c r="AG93" s="1"/>
-      <c r="AH93" s="1"/>
-      <c r="AI93" s="1"/>
-      <c r="AJ93" s="1"/>
-      <c r="AK93" s="1"/>
-      <c r="AL93" s="1"/>
-      <c r="AM93" s="1"/>
-      <c r="AN93" s="1"/>
-      <c r="AO93" s="1"/>
-      <c r="AP93" s="1"/>
-      <c r="AQ93" s="1"/>
-      <c r="AR93" s="1"/>
-      <c r="AS93" s="1"/>
-      <c r="AT93" s="1"/>
-      <c r="AU93" s="1"/>
-      <c r="AV93" s="7"/>
-      <c r="AW93" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AX93" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AY93" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AZ93" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="BA93" s="1"/>
-      <c r="BB93" s="1"/>
-      <c r="BC93" s="1"/>
-      <c r="BD93" s="1"/>
-      <c r="BE93" s="1"/>
-      <c r="BF93" s="1"/>
-      <c r="BG93" s="7"/>
-      <c r="BH93" s="1"/>
-      <c r="BI93" s="1"/>
-      <c r="BJ93" s="1"/>
-      <c r="BK93" s="1"/>
-      <c r="BL93" s="1"/>
-      <c r="BM93" s="1">
-        <v>19</v>
-      </c>
-      <c r="BN93" s="1"/>
-      <c r="BO93" s="1"/>
-      <c r="BP93" s="1"/>
-      <c r="BQ93" s="2"/>
-      <c r="BR93" s="8"/>
-      <c r="BS93" s="8"/>
-      <c r="BT93" s="8"/>
-      <c r="BU93" s="1"/>
-      <c r="BV93" s="1"/>
-      <c r="BW93" s="1"/>
-      <c r="BX93" s="1"/>
-      <c r="BY93" s="1"/>
-      <c r="BZ93" s="9"/>
-      <c r="CA93" s="9"/>
-      <c r="CB93" s="10"/>
-      <c r="CC93" s="10"/>
-      <c r="CD93" s="10"/>
-      <c r="CE93" s="14"/>
-      <c r="CF93" s="15"/>
-      <c r="CG93" s="10"/>
-      <c r="CH93" s="10"/>
-      <c r="CI93" s="10"/>
-      <c r="CJ93" s="10"/>
-      <c r="CK93" s="16"/>
-    </row>
-    <row r="94" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="H94" s="1"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K94" s="16"/>
-      <c r="L94" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M94" s="16">
-        <v>157</v>
-      </c>
-      <c r="N94" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="O94" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="P94" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q94" s="1"/>
-      <c r="R94" s="1"/>
-      <c r="S94" s="1"/>
-      <c r="T94" s="1"/>
-      <c r="U94" s="1"/>
-      <c r="V94" s="1"/>
-      <c r="W94" s="1"/>
-      <c r="X94" s="1"/>
-      <c r="Y94" s="1"/>
-      <c r="Z94" s="1"/>
-      <c r="AA94" s="1"/>
-      <c r="AB94" s="1"/>
-      <c r="AC94" s="1"/>
-      <c r="AD94" s="1"/>
-      <c r="AE94" s="1"/>
-      <c r="AF94" s="1"/>
-      <c r="AG94" s="1"/>
-      <c r="AH94" s="1"/>
-      <c r="AI94" s="1"/>
-      <c r="AJ94" s="1"/>
-      <c r="AK94" s="1"/>
-      <c r="AL94" s="1"/>
-      <c r="AM94" s="1"/>
-      <c r="AN94" s="1"/>
-      <c r="AO94" s="1"/>
-      <c r="AP94" s="1"/>
-      <c r="AQ94" s="1"/>
-      <c r="AR94" s="1"/>
-      <c r="AS94" s="1"/>
-      <c r="AT94" s="1"/>
-      <c r="AU94" s="1"/>
-      <c r="AV94" s="7"/>
-      <c r="AW94" s="1"/>
-      <c r="AX94" s="1"/>
-      <c r="AY94" s="1"/>
-      <c r="AZ94" s="1"/>
-      <c r="BA94" s="1"/>
-      <c r="BB94" s="1"/>
-      <c r="BC94" s="1"/>
-      <c r="BD94" s="1"/>
-      <c r="BE94" s="1"/>
-      <c r="BF94" s="1"/>
-      <c r="BG94" s="7"/>
-      <c r="BH94" s="1"/>
-      <c r="BI94" s="1"/>
-      <c r="BJ94" s="1"/>
-      <c r="BK94" s="1"/>
-      <c r="BL94" s="1"/>
-      <c r="BM94" s="1"/>
-      <c r="BN94" s="1"/>
-      <c r="BO94" s="1"/>
-      <c r="BP94" s="1"/>
-      <c r="BQ94" s="2"/>
-      <c r="BR94" s="8"/>
-      <c r="BS94" s="8"/>
-      <c r="BT94" s="8"/>
-      <c r="BU94" s="1"/>
-      <c r="BV94" s="1"/>
-      <c r="BW94" s="1"/>
-      <c r="BX94" s="1"/>
-      <c r="BY94" s="1"/>
-      <c r="BZ94" s="9"/>
-      <c r="CA94" s="9"/>
-      <c r="CB94" s="10"/>
-      <c r="CC94" s="10"/>
-      <c r="CD94" s="10"/>
-      <c r="CE94" s="14"/>
-      <c r="CF94" s="15"/>
-      <c r="CG94" s="10"/>
-      <c r="CH94" s="10"/>
-      <c r="CI94" s="10"/>
-      <c r="CJ94" s="10"/>
-      <c r="CK94" s="16"/>
-    </row>
-    <row r="95" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="H95" s="1"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K95" s="16"/>
-      <c r="L95" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M95" s="16">
-        <v>157</v>
-      </c>
-      <c r="N95" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="O95" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="P95" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="Q95" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="R95" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="S95" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="T95" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="U95" s="1"/>
-      <c r="V95" s="1"/>
-      <c r="W95" s="1"/>
-      <c r="X95" s="1"/>
-      <c r="Y95" s="1"/>
-      <c r="Z95" s="1"/>
-      <c r="AA95" s="1"/>
-      <c r="AB95" s="1"/>
-      <c r="AC95" s="1"/>
-      <c r="AD95" s="1"/>
-      <c r="AE95" s="1"/>
-      <c r="AF95" s="1"/>
-      <c r="AG95" s="1"/>
-      <c r="AH95" s="1"/>
-      <c r="AI95" s="1"/>
-      <c r="AJ95" s="1"/>
-      <c r="AK95" s="1"/>
-      <c r="AL95" s="1"/>
-      <c r="AM95" s="1"/>
-      <c r="AN95" s="1"/>
-      <c r="AO95" s="1"/>
-      <c r="AP95" s="1"/>
-      <c r="AQ95" s="1"/>
-      <c r="AR95" s="1"/>
-      <c r="AS95" s="1"/>
-      <c r="AT95" s="1"/>
-      <c r="AU95" s="1"/>
-      <c r="AV95" s="7"/>
-      <c r="AW95" s="1"/>
-      <c r="AX95" s="1"/>
-      <c r="AY95" s="1"/>
-      <c r="AZ95" s="1"/>
-      <c r="BA95" s="1"/>
-      <c r="BB95" s="1"/>
-      <c r="BC95" s="1"/>
-      <c r="BD95" s="1"/>
-      <c r="BE95" s="1"/>
-      <c r="BF95" s="1"/>
-      <c r="BG95" s="7"/>
-      <c r="BH95" s="1"/>
-      <c r="BI95" s="1"/>
-      <c r="BJ95" s="1"/>
-      <c r="BK95" s="1"/>
-      <c r="BL95" s="1"/>
-      <c r="BM95" s="1"/>
-      <c r="BN95" s="1"/>
-      <c r="BO95" s="1"/>
-      <c r="BP95" s="1"/>
-      <c r="BQ95" s="2"/>
-      <c r="BR95" s="8"/>
-      <c r="BS95" s="8"/>
-      <c r="BT95" s="8"/>
-      <c r="BU95" s="1"/>
-      <c r="BV95" s="1"/>
-      <c r="BW95" s="1"/>
-      <c r="BX95" s="1"/>
-      <c r="BY95" s="1"/>
-      <c r="BZ95" s="9"/>
-      <c r="CA95" s="9"/>
-      <c r="CB95" s="10"/>
-      <c r="CC95" s="10"/>
-      <c r="CD95" s="10"/>
-      <c r="CE95" s="14"/>
-      <c r="CF95" s="15"/>
-      <c r="CG95" s="10"/>
-      <c r="CH95" s="10"/>
-      <c r="CI95" s="10"/>
-      <c r="CJ95" s="10"/>
-      <c r="CK95" s="16"/>
-    </row>
-    <row r="96" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="H96" s="1"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K96" s="16"/>
-      <c r="L96" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M96" s="16">
-        <v>157</v>
-      </c>
-      <c r="N96" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="O96" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="P96" s="1"/>
-      <c r="Q96" s="1"/>
-      <c r="R96" s="1"/>
-      <c r="S96" s="1"/>
-      <c r="T96" s="1"/>
-      <c r="U96" s="1"/>
-      <c r="V96" s="1"/>
-      <c r="W96" s="1"/>
-      <c r="X96" s="1"/>
-      <c r="Y96" s="1"/>
-      <c r="Z96" s="1"/>
-      <c r="AA96" s="1"/>
-      <c r="AB96" s="1"/>
-      <c r="AC96" s="1"/>
-      <c r="AD96" s="1"/>
-      <c r="AE96" s="1"/>
-      <c r="AF96" s="1"/>
-      <c r="AG96" s="1"/>
-      <c r="AH96" s="1"/>
-      <c r="AI96" s="1"/>
-      <c r="AJ96" s="1"/>
-      <c r="AK96" s="1"/>
-      <c r="AL96" s="1"/>
-      <c r="AM96" s="1"/>
-      <c r="AN96" s="1"/>
-      <c r="AO96" s="1"/>
-      <c r="AP96" s="1"/>
-      <c r="AQ96" s="1"/>
-      <c r="AR96" s="1"/>
-      <c r="AS96" s="1"/>
-      <c r="AT96" s="1"/>
-      <c r="AU96" s="1"/>
-      <c r="AV96" s="7"/>
-      <c r="AW96" s="1"/>
-      <c r="AX96" s="1"/>
-      <c r="AY96" s="1"/>
-      <c r="AZ96" s="1"/>
-      <c r="BA96" s="1"/>
-      <c r="BB96" s="1"/>
-      <c r="BC96" s="1"/>
-      <c r="BD96" s="1"/>
-      <c r="BE96" s="1"/>
-      <c r="BF96" s="1"/>
-      <c r="BG96" s="7"/>
-      <c r="BH96" s="1"/>
-      <c r="BI96" s="1"/>
-      <c r="BJ96" s="1"/>
-      <c r="BK96" s="1"/>
-      <c r="BL96" s="1"/>
-      <c r="BM96" s="1"/>
-      <c r="BN96" s="1"/>
-      <c r="BO96" s="1"/>
-      <c r="BP96" s="1"/>
-      <c r="BQ96" s="2"/>
-      <c r="BR96" s="8"/>
-      <c r="BS96" s="8"/>
-      <c r="BT96" s="8"/>
-      <c r="BU96" s="1"/>
-      <c r="BV96" s="1"/>
-      <c r="BW96" s="1"/>
-      <c r="BX96" s="1"/>
-      <c r="BY96" s="1"/>
-      <c r="BZ96" s="9"/>
-      <c r="CA96" s="9"/>
-      <c r="CB96" s="10"/>
-      <c r="CC96" s="10"/>
-      <c r="CD96" s="10"/>
-      <c r="CE96" s="14"/>
-      <c r="CF96" s="15"/>
-      <c r="CG96" s="10"/>
-      <c r="CH96" s="10"/>
-      <c r="CI96" s="10"/>
-      <c r="CJ96" s="10"/>
-      <c r="CK96" s="16"/>
-    </row>
-    <row r="97" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="H97" s="1"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K97" s="16"/>
-      <c r="L97" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M97" s="16">
-        <v>157</v>
-      </c>
-      <c r="N97" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="O97" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="P97" s="1"/>
-      <c r="Q97" s="1"/>
-      <c r="R97" s="1"/>
-      <c r="S97" s="1"/>
-      <c r="T97" s="1"/>
-      <c r="U97" s="1"/>
-      <c r="V97" s="1"/>
-      <c r="W97" s="1"/>
-      <c r="X97" s="1"/>
-      <c r="Y97" s="1"/>
-      <c r="Z97" s="1"/>
-      <c r="AA97" s="1"/>
-      <c r="AB97" s="1"/>
-      <c r="AC97" s="1"/>
-      <c r="AD97" s="1"/>
-      <c r="AE97" s="1"/>
-      <c r="AF97" s="1"/>
-      <c r="AG97" s="1"/>
-      <c r="AH97" s="1"/>
-      <c r="AI97" s="1"/>
-      <c r="AJ97" s="1"/>
-      <c r="AK97" s="1"/>
-      <c r="AL97" s="1"/>
-      <c r="AM97" s="1"/>
-      <c r="AN97" s="1"/>
-      <c r="AO97" s="1"/>
-      <c r="AP97" s="1"/>
-      <c r="AQ97" s="1"/>
-      <c r="AR97" s="1"/>
-      <c r="AS97" s="1"/>
-      <c r="AT97" s="1"/>
-      <c r="AU97" s="1"/>
-      <c r="AV97" s="7"/>
-      <c r="AW97" s="1"/>
-      <c r="AX97" s="1"/>
-      <c r="AY97" s="1"/>
-      <c r="AZ97" s="1"/>
-      <c r="BA97" s="1"/>
-      <c r="BB97" s="1"/>
-      <c r="BC97" s="1"/>
-      <c r="BD97" s="1"/>
-      <c r="BE97" s="1"/>
-      <c r="BF97" s="1"/>
-      <c r="BG97" s="7"/>
-      <c r="BH97" s="1"/>
-      <c r="BI97" s="1"/>
-      <c r="BJ97" s="1"/>
-      <c r="BK97" s="1"/>
-      <c r="BL97" s="1"/>
-      <c r="BM97" s="1"/>
-      <c r="BN97" s="1"/>
-      <c r="BO97" s="1"/>
-      <c r="BP97" s="1"/>
-      <c r="BQ97" s="2"/>
-      <c r="BR97" s="8"/>
-      <c r="BS97" s="8"/>
-      <c r="BT97" s="8"/>
-      <c r="BU97" s="1"/>
-      <c r="BV97" s="1"/>
-      <c r="BW97" s="1"/>
-      <c r="BX97" s="1"/>
-      <c r="BY97" s="1"/>
-      <c r="BZ97" s="9"/>
-      <c r="CA97" s="9"/>
-      <c r="CB97" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="CC97" s="10"/>
-      <c r="CD97" s="10"/>
-      <c r="CE97" s="14"/>
-      <c r="CF97" s="15"/>
-      <c r="CG97" s="10"/>
-      <c r="CH97" s="10"/>
-      <c r="CI97" s="10"/>
-      <c r="CJ97" s="10"/>
-      <c r="CK97" s="16"/>
-    </row>
-    <row r="98" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="H98" s="1"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K98" s="16"/>
-      <c r="L98" s="16" t="s">
-        <v>543</v>
-      </c>
-      <c r="M98" s="16">
-        <v>158</v>
-      </c>
-      <c r="N98" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="O98" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1"/>
-      <c r="U98" s="1"/>
-      <c r="V98" s="1"/>
-      <c r="W98" s="1"/>
-      <c r="X98" s="1"/>
-      <c r="Y98" s="1"/>
-      <c r="Z98" s="1"/>
-      <c r="AA98" s="1"/>
-      <c r="AB98" s="1"/>
-      <c r="AC98" s="1"/>
-      <c r="AD98" s="1"/>
-      <c r="AE98" s="1"/>
-      <c r="AF98" s="1"/>
-      <c r="AG98" s="1"/>
-      <c r="AH98" s="1"/>
-      <c r="AI98" s="1"/>
-      <c r="AJ98" s="1"/>
-      <c r="AK98" s="1"/>
-      <c r="AL98" s="1"/>
-      <c r="AM98" s="1"/>
-      <c r="AN98" s="1"/>
-      <c r="AO98" s="1"/>
-      <c r="AP98" s="1"/>
-      <c r="AQ98" s="1"/>
-      <c r="AR98" s="1"/>
-      <c r="AS98" s="1"/>
-      <c r="AT98" s="1"/>
-      <c r="AU98" s="1"/>
-      <c r="AV98" s="7"/>
-      <c r="AW98" s="1"/>
-      <c r="AX98" s="1"/>
-      <c r="AY98" s="1"/>
-      <c r="AZ98" s="1"/>
-      <c r="BA98" s="1"/>
-      <c r="BB98" s="1"/>
-      <c r="BC98" s="1"/>
-      <c r="BD98" s="1"/>
-      <c r="BE98" s="1"/>
-      <c r="BF98" s="1"/>
-      <c r="BG98" s="7"/>
-      <c r="BH98" s="1"/>
-      <c r="BI98" s="1"/>
-      <c r="BJ98" s="1"/>
-      <c r="BK98" s="1"/>
-      <c r="BL98" s="1"/>
-      <c r="BM98" s="1"/>
-      <c r="BN98" s="1"/>
-      <c r="BO98" s="1"/>
-      <c r="BP98" s="1"/>
-      <c r="BQ98" s="2"/>
-      <c r="BR98" s="8"/>
-      <c r="BS98" s="8"/>
-      <c r="BT98" s="8"/>
-      <c r="BU98" s="1"/>
-      <c r="BV98" s="1"/>
-      <c r="BW98" s="1"/>
-      <c r="BX98" s="1"/>
-      <c r="BY98" s="1"/>
-      <c r="BZ98" s="9"/>
-      <c r="CA98" s="9"/>
-      <c r="CB98" s="10"/>
-      <c r="CC98" s="10"/>
-      <c r="CD98" s="10"/>
-      <c r="CE98" s="14"/>
-      <c r="CF98" s="15"/>
-      <c r="CG98" s="10"/>
-      <c r="CH98" s="10"/>
-      <c r="CI98" s="10"/>
-      <c r="CJ98" s="10"/>
-      <c r="CK98" s="16"/>
-    </row>
-    <row r="99" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="H99" s="1"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K99" s="16"/>
-      <c r="L99" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M99" s="16">
-        <v>157</v>
-      </c>
-      <c r="N99" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="O99" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
-      <c r="R99" s="1"/>
-      <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
-      <c r="U99" s="1"/>
-      <c r="V99" s="1"/>
-      <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
-      <c r="Y99" s="1"/>
-      <c r="Z99" s="1"/>
-      <c r="AA99" s="1"/>
-      <c r="AB99" s="1"/>
-      <c r="AC99" s="1"/>
-      <c r="AD99" s="1"/>
-      <c r="AE99" s="1"/>
-      <c r="AF99" s="1"/>
-      <c r="AG99" s="1"/>
-      <c r="AH99" s="1"/>
-      <c r="AI99" s="1"/>
-      <c r="AJ99" s="1"/>
-      <c r="AK99" s="1"/>
-      <c r="AL99" s="1"/>
-      <c r="AM99" s="1"/>
-      <c r="AN99" s="1"/>
-      <c r="AO99" s="1"/>
-      <c r="AP99" s="1"/>
-      <c r="AQ99" s="1"/>
-      <c r="AR99" s="1"/>
-      <c r="AS99" s="1"/>
-      <c r="AT99" s="1"/>
-      <c r="AU99" s="1"/>
-      <c r="AV99" s="7"/>
-      <c r="AW99" s="1"/>
-      <c r="AX99" s="1"/>
-      <c r="AY99" s="1"/>
-      <c r="AZ99" s="1"/>
-      <c r="BA99" s="1"/>
-      <c r="BB99" s="1"/>
-      <c r="BC99" s="1"/>
-      <c r="BD99" s="1"/>
-      <c r="BE99" s="1"/>
-      <c r="BF99" s="1"/>
-      <c r="BG99" s="7"/>
-      <c r="BH99" s="1"/>
-      <c r="BI99" s="1"/>
-      <c r="BJ99" s="1"/>
-      <c r="BK99" s="1"/>
-      <c r="BL99" s="1"/>
-      <c r="BM99" s="1"/>
-      <c r="BN99" s="1"/>
-      <c r="BO99" s="1"/>
-      <c r="BP99" s="1"/>
-      <c r="BQ99" s="2"/>
-      <c r="BR99" s="8"/>
-      <c r="BS99" s="8"/>
-      <c r="BT99" s="8"/>
-      <c r="BU99" s="1"/>
-      <c r="BV99" s="1"/>
-      <c r="BW99" s="1"/>
-      <c r="BX99" s="1"/>
-      <c r="BY99" s="1"/>
-      <c r="BZ99" s="9"/>
-      <c r="CA99" s="9"/>
-      <c r="CB99" s="10"/>
-      <c r="CC99" s="10"/>
-      <c r="CD99" s="10"/>
-      <c r="CE99" s="14"/>
-      <c r="CF99" s="15"/>
-      <c r="CG99" s="10"/>
-      <c r="CH99" s="10"/>
-      <c r="CI99" s="10"/>
-      <c r="CJ99" s="10"/>
-      <c r="CK99" s="16"/>
-    </row>
-    <row r="100" spans="1:89" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="H100" s="1"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="K100" s="16"/>
-      <c r="L100" s="16" t="s">
-        <v>480</v>
-      </c>
-      <c r="M100" s="16">
-        <v>157</v>
-      </c>
-      <c r="N100" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="O100" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
-      <c r="R100" s="1"/>
-      <c r="S100" s="1"/>
-      <c r="T100" s="1"/>
-      <c r="U100" s="1"/>
-      <c r="V100" s="1"/>
-      <c r="W100" s="1"/>
-      <c r="X100" s="1"/>
-      <c r="Y100" s="1"/>
-      <c r="Z100" s="1"/>
-      <c r="AA100" s="1"/>
-      <c r="AB100" s="1"/>
-      <c r="AC100" s="1"/>
-      <c r="AD100" s="1"/>
-      <c r="AE100" s="1"/>
-      <c r="AF100" s="1"/>
-      <c r="AG100" s="1"/>
-      <c r="AH100" s="1"/>
-      <c r="AI100" s="1"/>
-      <c r="AJ100" s="1"/>
-      <c r="AK100" s="1"/>
-      <c r="AL100" s="1"/>
-      <c r="AM100" s="1"/>
-      <c r="AN100" s="1"/>
-      <c r="AO100" s="1"/>
-      <c r="AP100" s="1"/>
-      <c r="AQ100" s="1"/>
-      <c r="AR100" s="1"/>
-      <c r="AS100" s="1"/>
-      <c r="AT100" s="1"/>
-      <c r="AU100" s="1"/>
-      <c r="AV100" s="7"/>
-      <c r="AW100" s="1"/>
-      <c r="AX100" s="1"/>
-      <c r="AY100" s="1"/>
-      <c r="AZ100" s="1"/>
-      <c r="BA100" s="1"/>
-      <c r="BB100" s="1"/>
-      <c r="BC100" s="1"/>
-      <c r="BD100" s="1"/>
-      <c r="BE100" s="1"/>
-      <c r="BF100" s="1"/>
-      <c r="BG100" s="7"/>
-      <c r="BH100" s="1"/>
-      <c r="BI100" s="1"/>
-      <c r="BJ100" s="1"/>
-      <c r="BK100" s="1"/>
-      <c r="BL100" s="1"/>
-      <c r="BM100" s="1"/>
-      <c r="BN100" s="1"/>
-      <c r="BO100" s="1"/>
-      <c r="BP100" s="1"/>
-      <c r="BQ100" s="2"/>
-      <c r="BR100" s="8"/>
-      <c r="BS100" s="8"/>
-      <c r="BT100" s="8"/>
-      <c r="BU100" s="1"/>
-      <c r="BV100" s="1"/>
-      <c r="BW100" s="1"/>
-      <c r="BX100" s="1"/>
-      <c r="BY100" s="1"/>
-      <c r="BZ100" s="9"/>
-      <c r="CA100" s="9"/>
-      <c r="CB100" s="10"/>
-      <c r="CC100" s="10"/>
-      <c r="CD100" s="10"/>
-      <c r="CE100" s="14"/>
-      <c r="CF100" s="15"/>
-      <c r="CG100" s="10"/>
-      <c r="CH100" s="10"/>
-      <c r="CI100" s="10"/>
-      <c r="CJ100" s="10"/>
-      <c r="CK100" s="16"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Fixed quota issue and survey download issue
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
+++ b/Engage/Sogo-Performance/src/main/resources/excelfiles/Sogo_PlatformReadings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BF56FF-CEEF-481C-9985-C9FA88E9D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A1A4C7-F22A-490F-B86D-33FB16027D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="584">
   <si>
     <t>Environment</t>
   </si>
@@ -1772,6 +1772,9 @@
   </si>
   <si>
     <t>Rearrange 10 questions - save  (sid - 157)</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -1779,7 +1782,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1866,7 +1869,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1891,11 +1893,16 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <u val="single"/>
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1971,17 +1978,47 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2069,7 +2106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2103,7 +2140,10 @@
     <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="17" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2613,7 +2653,7 @@
   <dimension ref="A1:CK91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N95" sqref="N95"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10399,7 +10439,7 @@
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="11"/>
-      <c r="J62" s="26" t="s">
+      <c r="J62" s="25" t="s">
         <v>26</v>
       </c>
       <c r="K62" s="16"/>
@@ -12818,7 +12858,7 @@
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="11"/>
-      <c r="J83" s="28" t="s">
+      <c r="J83" s="26" t="s">
         <v>515</v>
       </c>
       <c r="K83" s="16"/>
@@ -13296,7 +13336,7 @@
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="11"/>
-      <c r="J87" s="25" t="s">
+      <c r="J87" s="24" t="s">
         <v>515</v>
       </c>
       <c r="K87" s="16"/>
@@ -13517,7 +13557,7 @@
         <v>574</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>21</v>
@@ -13536,7 +13576,7 @@
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="11"/>
-      <c r="J89" s="24" t="s">
+      <c r="J89" s="27" t="s">
         <v>515</v>
       </c>
       <c r="K89" s="16"/>
@@ -13751,7 +13791,7 @@
         <v>578</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>21</v>
@@ -13770,8 +13810,8 @@
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="11"/>
-      <c r="J91" s="21" t="s">
-        <v>26</v>
+      <c r="J91" s="31" t="s">
+        <v>515</v>
       </c>
       <c r="K91" s="16"/>
       <c r="L91" s="16" t="s">

</xml_diff>